<commit_message>
Use architect's door annotations (kapi-yazi) for exact dimensions
Door sizes now come from architect's text annotations on kapi-yazi
layer (90/220, 100/220, 200/220) instead of xscale-derived values
(880, 980, 1980) which were slightly off from intended dimensions.

Result: 900x2200, 1000x2200, 2000x2200 — 413 doors, 658 total openings.

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/resources/AL_KABIR_TOWER_Opening_Schedule.xlsx
+++ b/resources/AL_KABIR_TOWER_Opening_Schedule.xlsx
@@ -84,13 +84,13 @@
     <t>Total Doors:</t>
   </si>
   <si>
-    <t>422</t>
+    <t>413</t>
   </si>
   <si>
     <t>Total Openings:</t>
   </si>
   <si>
-    <t>667</t>
+    <t>658</t>
   </si>
   <si>
     <t>Window Area:</t>
@@ -102,13 +102,13 @@
     <t>Door Area:</t>
   </si>
   <si>
-    <t>854.4 m²</t>
+    <t>855.1 m²</t>
   </si>
   <si>
     <t>Total Facade Area:</t>
   </si>
   <si>
-    <t>1799.1 m²</t>
+    <t>1799.8 m²</t>
   </si>
   <si>
     <t>ALL OPENINGS OVERVIEW</t>
@@ -349,7 +349,7 @@
     <t>WINDOWS (9 types, 245 units)</t>
   </si>
   <si>
-    <t>DOORS (3 types, 422 units)</t>
+    <t>DOORS (3 types, 413 units)</t>
   </si>
   <si>
     <t>GRAND TOTAL FACADE AREA</t>
@@ -415,13 +415,13 @@
     <t>WINDOW TOTAL</t>
   </si>
   <si>
-    <t>Single Leaf Hinged Door 880mm</t>
-  </si>
-  <si>
-    <t>Single Leaf Hinged Door 980mm</t>
-  </si>
-  <si>
-    <t>Double Leaf Hinged Entrance Door 1980mm</t>
+    <t>Single Leaf Hinged Door 900mm</t>
+  </si>
+  <si>
+    <t>Single Leaf Hinged Door 1000mm</t>
+  </si>
+  <si>
+    <t>Double Leaf Hinged Entrance Door 2000mm</t>
   </si>
   <si>
     <t>DOOR TOTAL</t>
@@ -1706,7 +1706,7 @@
         <v>55</v>
       </c>
       <c r="D36" s="15">
-        <v>880</v>
+        <v>900</v>
       </c>
       <c r="E36" s="15">
         <v>2200</v>
@@ -1715,13 +1715,13 @@
         <v>56</v>
       </c>
       <c r="G36" s="15">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="H36" s="16">
-        <v>1.94</v>
+        <v>1.98</v>
       </c>
       <c r="I36" s="17">
-        <v>700.8</v>
+        <v>698.9</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -1735,7 +1735,7 @@
         <v>55</v>
       </c>
       <c r="D37" s="10">
-        <v>980</v>
+        <v>1000</v>
       </c>
       <c r="E37" s="10">
         <v>2200</v>
@@ -1747,10 +1747,10 @@
         <v>49</v>
       </c>
       <c r="H37" s="11">
-        <v>2.16</v>
+        <v>2.2</v>
       </c>
       <c r="I37" s="12">
-        <v>105.6</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1764,7 +1764,7 @@
         <v>55</v>
       </c>
       <c r="D38" s="15">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="E38" s="15">
         <v>2200</v>
@@ -1776,10 +1776,10 @@
         <v>11</v>
       </c>
       <c r="H38" s="16">
-        <v>4.36</v>
+        <v>4.4</v>
       </c>
       <c r="I38" s="17">
-        <v>47.9</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1792,11 +1792,11 @@
       <c r="E39" s="18"/>
       <c r="F39" s="18"/>
       <c r="G39" s="20">
-        <v>667</v>
+        <v>658</v>
       </c>
       <c r="H39" s="18"/>
       <c r="I39" s="21">
-        <v>1799.1</v>
+        <v>1799.8</v>
       </c>
     </row>
   </sheetData>
@@ -2381,7 +2381,7 @@
         <v>54</v>
       </c>
       <c r="C6" s="15">
-        <v>880</v>
+        <v>900</v>
       </c>
       <c r="D6" s="15">
         <v>2200</v>
@@ -2390,19 +2390,19 @@
         <v>56</v>
       </c>
       <c r="F6" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="13">
         <v>20</v>
       </c>
       <c r="H6" s="15">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="I6" s="16">
-        <v>1.94</v>
+        <v>1.98</v>
       </c>
       <c r="J6" s="17">
-        <v>700.8</v>
+        <v>698.9</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -2413,7 +2413,7 @@
         <v>57</v>
       </c>
       <c r="C7" s="10">
-        <v>980</v>
+        <v>1000</v>
       </c>
       <c r="D7" s="10">
         <v>2200</v>
@@ -2431,10 +2431,10 @@
         <v>49</v>
       </c>
       <c r="I7" s="11">
-        <v>2.16</v>
+        <v>2.2</v>
       </c>
       <c r="J7" s="12">
-        <v>105.6</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2445,7 +2445,7 @@
         <v>58</v>
       </c>
       <c r="C8" s="15">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="D8" s="15">
         <v>2200</v>
@@ -2463,10 +2463,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="16">
-        <v>4.36</v>
+        <v>4.4</v>
       </c>
       <c r="J8" s="17">
-        <v>47.9</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -2478,17 +2478,17 @@
         <v>87</v>
       </c>
       <c r="F9" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G9" s="25">
         <v>26</v>
       </c>
       <c r="H9" s="25">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="I9" s="23"/>
       <c r="J9" s="26">
-        <v>854.4</v>
+        <v>855.1</v>
       </c>
     </row>
   </sheetData>
@@ -3093,43 +3093,43 @@
         <v>56</v>
       </c>
       <c r="D18" s="15">
-        <v>880</v>
+        <v>900</v>
       </c>
       <c r="E18" s="15">
         <v>2200</v>
       </c>
       <c r="F18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N18" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" s="13">
         <v>20</v>
       </c>
       <c r="P18" s="15">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -3143,7 +3143,7 @@
         <v>56</v>
       </c>
       <c r="D19" s="10">
-        <v>980</v>
+        <v>1000</v>
       </c>
       <c r="E19" s="10">
         <v>2200</v>
@@ -3193,7 +3193,7 @@
         <v>59</v>
       </c>
       <c r="D20" s="15">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="E20" s="15">
         <v>2200</v>
@@ -3241,37 +3241,37 @@
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
       <c r="F21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N21" s="25">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O21" s="25">
         <v>26</v>
       </c>
       <c r="P21" s="25">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -3283,37 +3283,37 @@
       <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="I22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N22" s="20">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O22" s="20">
         <v>46</v>
       </c>
       <c r="P22" s="20">
-        <v>667</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>
@@ -3670,19 +3670,19 @@
         <v>56</v>
       </c>
       <c r="D20" s="15">
-        <v>880</v>
+        <v>900</v>
       </c>
       <c r="E20" s="15">
         <v>2200</v>
       </c>
       <c r="F20" s="16">
-        <v>1.94</v>
+        <v>1.98</v>
       </c>
       <c r="G20" s="15">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="H20" s="17">
-        <v>700.8</v>
+        <v>698.9</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -3696,19 +3696,19 @@
         <v>56</v>
       </c>
       <c r="D21" s="10">
-        <v>980</v>
+        <v>1000</v>
       </c>
       <c r="E21" s="10">
         <v>2200</v>
       </c>
       <c r="F21" s="11">
-        <v>2.16</v>
+        <v>2.2</v>
       </c>
       <c r="G21" s="10">
         <v>49</v>
       </c>
       <c r="H21" s="12">
-        <v>105.6</v>
+        <v>107.8</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -3722,19 +3722,19 @@
         <v>59</v>
       </c>
       <c r="D22" s="15">
-        <v>1980</v>
+        <v>2000</v>
       </c>
       <c r="E22" s="15">
         <v>2200</v>
       </c>
       <c r="F22" s="16">
-        <v>4.36</v>
+        <v>4.4</v>
       </c>
       <c r="G22" s="15">
         <v>11</v>
       </c>
       <c r="H22" s="17">
-        <v>47.9</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -3747,10 +3747,10 @@
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="25">
-        <v>422</v>
+        <v>413</v>
       </c>
       <c r="H23" s="26">
-        <v>854.3</v>
+        <v>855.1</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -3763,10 +3763,10 @@
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="20">
-        <v>667</v>
+        <v>658</v>
       </c>
       <c r="H24" s="21">
-        <v>1798.9</v>
+        <v>1799.7</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4344,7 @@
         <v>119</v>
       </c>
       <c r="D30" s="13">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>114</v>
@@ -4357,7 +4357,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="15">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="I30" s="13"/>
     </row>
@@ -4383,7 +4383,7 @@
         <v>20</v>
       </c>
       <c r="I31" s="25">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="2:9">
@@ -4497,7 +4497,7 @@
       <c r="G36" s="23"/>
       <c r="H36" s="23"/>
       <c r="I36" s="25">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="37" spans="2:9">
@@ -4511,7 +4511,7 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
       <c r="I37" s="20">
-        <v>667</v>
+        <v>658</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct opening names: Sliding Door (h>=2200) vs Sliding Window
All openings are sliding — no fixed glass or top hung in this project.
- Height >= 2200mm = Sliding Door (floor-to-ceiling balcony access)
- Height < 2200mm = Sliding Window (600x600 bathroom, 2200x1500 landscape)
- Panel count from width: >=2400mm = 4P, >=1200mm = 3P, else 2P

Co-Authored-By: Claude Opus 4.6 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/resources/AL_KABIR_TOWER_Opening_Schedule.xlsx
+++ b/resources/AL_KABIR_TOWER_Opening_Schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="133">
   <si>
     <t>AL KABIR TOWER</t>
   </si>
@@ -147,13 +147,13 @@
     <t>Window</t>
   </si>
   <si>
-    <t>Top Hung Window (1P)</t>
+    <t>2-Panel Sliding Window (2P)</t>
   </si>
   <si>
     <t>W02</t>
   </si>
   <si>
-    <t>Fixed Window (1P)</t>
+    <t>3-Panel Sliding Door (3P)</t>
   </si>
   <si>
     <t>W03</t>
@@ -165,22 +165,22 @@
     <t>W05</t>
   </si>
   <si>
+    <t>W06</t>
+  </si>
+  <si>
+    <t>W07</t>
+  </si>
+  <si>
     <t>3-Panel Sliding Window (3P)</t>
   </si>
   <si>
-    <t>W06</t>
-  </si>
-  <si>
-    <t>W07</t>
-  </si>
-  <si>
     <t>W08</t>
   </si>
   <si>
     <t>W09</t>
   </si>
   <si>
-    <t>4-Panel Sliding Window (4P)</t>
+    <t>4-Panel Sliding Door (4P)</t>
   </si>
   <si>
     <t>D01</t>
@@ -232,19 +232,16 @@
 Qty</t>
   </si>
   <si>
-    <t>Top Hung Window</t>
-  </si>
-  <si>
-    <t>Top Hung</t>
+    <t>2-Panel Sliding Window</t>
+  </si>
+  <si>
+    <t>Horizontal Sliding</t>
   </si>
   <si>
     <t>E2×2, E2×4</t>
   </si>
   <si>
-    <t>Fixed Window</t>
-  </si>
-  <si>
-    <t>Fixed</t>
+    <t>3-Panel Sliding Door</t>
   </si>
   <si>
     <t>E1×2</t>
@@ -256,22 +253,19 @@
     <t>E3×1, E4×1</t>
   </si>
   <si>
+    <t>E1×4, E3×1, E4×1</t>
+  </si>
+  <si>
+    <t>E1×3</t>
+  </si>
+  <si>
     <t>3-Panel Sliding Window</t>
   </si>
   <si>
-    <t>Horizontal Sliding</t>
-  </si>
-  <si>
-    <t>E1×4, E3×1, E4×1</t>
-  </si>
-  <si>
-    <t>E1×3</t>
-  </si>
-  <si>
     <t>E2×2, E3×1, E4×1, E1×2, E2×2, E3×2, E4×2</t>
   </si>
   <si>
-    <t>4-Panel Sliding Window</t>
+    <t>4-Panel Sliding Door</t>
   </si>
   <si>
     <t>E3×2, E4×2, E1×4</t>
@@ -379,7 +373,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Top Hung Window 600×600mm</t>
+    <t>2-Panel Sliding Window 600×600mm</t>
   </si>
   <si>
     <t>RST FLOOR</t>
@@ -388,28 +382,28 @@
     <t>LAST</t>
   </si>
   <si>
-    <t>Fixed Window 1200×2200mm</t>
-  </si>
-  <si>
-    <t>Fixed Window 1500×2200mm</t>
-  </si>
-  <si>
-    <t>Fixed Window 1600×2200mm</t>
-  </si>
-  <si>
-    <t>3-Panel Sliding Window 1800×2200mm</t>
-  </si>
-  <si>
-    <t>3-Panel Sliding Window 2000×2200mm</t>
+    <t>3-Panel Sliding Door 1200×2200mm</t>
+  </si>
+  <si>
+    <t>3-Panel Sliding Door 1500×2200mm</t>
+  </si>
+  <si>
+    <t>3-Panel Sliding Door 1600×2200mm</t>
+  </si>
+  <si>
+    <t>3-Panel Sliding Door 1800×2200mm</t>
+  </si>
+  <si>
+    <t>3-Panel Sliding Door 2000×2200mm</t>
   </si>
   <si>
     <t>3-Panel Sliding Window 2200×1500mm</t>
   </si>
   <si>
-    <t>3-Panel Sliding Window 2200×2200mm</t>
-  </si>
-  <si>
-    <t>4-Panel Sliding Window 2400×2200mm</t>
+    <t>3-Panel Sliding Door 2200×2200mm</t>
+  </si>
+  <si>
+    <t>4-Panel Sliding Door 2400×2200mm</t>
   </si>
   <si>
     <t>WINDOW TOTAL</t>
@@ -1567,7 +1561,7 @@
         <v>2200</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G31" s="10">
         <v>54</v>
@@ -1584,7 +1578,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>41</v>
@@ -1596,7 +1590,7 @@
         <v>2200</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G32" s="15">
         <v>27</v>
@@ -1613,7 +1607,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>41</v>
@@ -1625,7 +1619,7 @@
         <v>1500</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G33" s="10">
         <v>2</v>
@@ -1654,7 +1648,7 @@
         <v>2200</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G34" s="15">
         <v>44</v>
@@ -1929,7 +1923,7 @@
         <v>69</v>
       </c>
       <c r="F7" s="13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="14" t="s">
         <v>70</v>
@@ -1970,13 +1964,13 @@
         <v>72</v>
       </c>
       <c r="F8" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="9" t="s">
         <v>73</v>
-      </c>
-      <c r="H8" s="9" t="s">
-        <v>74</v>
       </c>
       <c r="I8" s="8">
         <v>2</v>
@@ -2009,13 +2003,13 @@
         <v>72</v>
       </c>
       <c r="F9" s="13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I9" s="13">
         <v>4</v>
@@ -2048,13 +2042,13 @@
         <v>72</v>
       </c>
       <c r="F10" s="8">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8">
@@ -2084,16 +2078,16 @@
         <v>2200</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F11" s="13">
         <v>3</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I11" s="13">
         <v>6</v>
@@ -2114,7 +2108,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="10">
         <v>2000</v>
@@ -2123,16 +2117,16 @@
         <v>2200</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F12" s="8">
         <v>3</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I12" s="8">
         <v>3</v>
@@ -2153,7 +2147,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="15">
         <v>2200</v>
@@ -2162,16 +2156,16 @@
         <v>1500</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F13" s="13">
         <v>3</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I13" s="13"/>
       <c r="J13" s="13">
@@ -2201,16 +2195,16 @@
         <v>2200</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F14" s="8">
         <v>3</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I14" s="8">
         <v>4</v>
@@ -2242,16 +2236,16 @@
         <v>2200</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F15" s="13">
         <v>4</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I15" s="13">
         <v>4</v>
@@ -2275,7 +2269,7 @@
       <c r="C16" s="23"/>
       <c r="D16" s="23"/>
       <c r="E16" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F16" s="23"/>
       <c r="G16" s="23"/>
@@ -2329,7 +2323,7 @@
   <sheetData>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2355,7 +2349,7 @@
         <v>35</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>66</v>
@@ -2475,7 +2469,7 @@
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F9" s="25">
         <v>43</v>
@@ -2526,7 +2520,7 @@
   <sheetData>
     <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2552,7 +2546,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>34</v>
@@ -2561,42 +2555,42 @@
         <v>35</v>
       </c>
       <c r="F5" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="I5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="K5" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="M5" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="M5" s="7" t="s">
+      <c r="O5" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="P5" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B6" s="27"/>
       <c r="C6" s="27"/>
@@ -2800,7 +2794,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D11" s="15">
         <v>1800</v>
@@ -2845,10 +2839,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D12" s="10">
         <v>2000</v>
@@ -2893,10 +2887,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D13" s="15">
         <v>2200</v>
@@ -2928,7 +2922,7 @@
         <v>51</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D14" s="10">
         <v>2200</v>
@@ -2978,7 +2972,7 @@
         <v>52</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D15" s="15">
         <v>2400</v>
@@ -3024,7 +3018,7 @@
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
@@ -3064,7 +3058,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="28"/>
@@ -3236,7 +3230,7 @@
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
@@ -3349,7 +3343,7 @@
   <sheetData>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -3367,7 +3361,7 @@
         <v>32</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>34</v>
@@ -3387,7 +3381,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B8" s="27"/>
       <c r="C8" s="27"/>
@@ -3509,7 +3503,7 @@
         <v>47</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D13" s="15">
         <v>1800</v>
@@ -3532,10 +3526,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D14" s="10">
         <v>2000</v>
@@ -3558,10 +3552,10 @@
         <v>7</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D15" s="15">
         <v>2200</v>
@@ -3587,7 +3581,7 @@
         <v>51</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D16" s="10">
         <v>2200</v>
@@ -3613,7 +3607,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D17" s="15">
         <v>2400</v>
@@ -3635,7 +3629,7 @@
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="23"/>
@@ -3649,7 +3643,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="28"/>
@@ -3741,7 +3735,7 @@
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="24" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
@@ -3757,7 +3751,7 @@
       <c r="A24" s="18"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D24" s="18"/>
       <c r="E24" s="18"/>
@@ -3799,7 +3793,7 @@
   <sheetData>
     <row r="5" spans="2:9">
       <c r="B5" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -3811,7 +3805,7 @@
     </row>
     <row r="6" spans="2:9">
       <c r="B6" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -3823,34 +3817,34 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F8" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="G8" s="7">
         <f/>
         <v>0</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
@@ -3862,16 +3856,16 @@
     </row>
     <row r="10" spans="2:9">
       <c r="B10" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" s="13">
         <v>2</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F10" s="13">
         <v>9</v>
@@ -3888,13 +3882,13 @@
     <row r="11" spans="2:9">
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D11" s="13">
         <v>4</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F11" s="13">
         <v>1</v>
@@ -3912,16 +3906,16 @@
     </row>
     <row r="12" spans="2:9">
       <c r="B12" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="8">
         <v>2</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F12" s="8">
         <v>9</v>
@@ -3938,13 +3932,13 @@
     <row r="13" spans="2:9">
       <c r="B13" s="9"/>
       <c r="C13" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D13" s="8">
         <v>0</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F13" s="8">
         <v>1</v>
@@ -3962,16 +3956,16 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="13">
         <v>4</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F14" s="13">
         <v>9</v>
@@ -3988,13 +3982,13 @@
     <row r="15" spans="2:9">
       <c r="B15" s="14"/>
       <c r="C15" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D15" s="13">
         <v>0</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F15" s="13">
         <v>1</v>
@@ -4012,16 +4006,16 @@
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D16" s="8">
         <v>0</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F16" s="8">
         <v>9</v>
@@ -4038,13 +4032,13 @@
     <row r="17" spans="2:9">
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D17" s="8">
         <v>2</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F17" s="8">
         <v>1</v>
@@ -4062,16 +4056,16 @@
     </row>
     <row r="18" spans="2:9">
       <c r="B18" s="14" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D18" s="13">
         <v>6</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F18" s="13">
         <v>9</v>
@@ -4088,13 +4082,13 @@
     <row r="19" spans="2:9">
       <c r="B19" s="14"/>
       <c r="C19" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D19" s="13">
         <v>0</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F19" s="13">
         <v>1</v>
@@ -4112,16 +4106,16 @@
     </row>
     <row r="20" spans="2:9">
       <c r="B20" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D20" s="8">
         <v>3</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F20" s="8">
         <v>9</v>
@@ -4138,13 +4132,13 @@
     <row r="21" spans="2:9">
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D21" s="8">
         <v>0</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F21" s="8">
         <v>1</v>
@@ -4162,16 +4156,16 @@
     </row>
     <row r="22" spans="2:9">
       <c r="B22" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D22" s="13">
         <v>0</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F22" s="13">
         <v>9</v>
@@ -4188,13 +4182,13 @@
     <row r="23" spans="2:9">
       <c r="B23" s="14"/>
       <c r="C23" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F23" s="13">
         <v>1</v>
@@ -4212,16 +4206,16 @@
     </row>
     <row r="24" spans="2:9">
       <c r="B24" s="9" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D24" s="8">
         <v>4</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F24" s="8">
         <v>9</v>
@@ -4238,13 +4232,13 @@
     <row r="25" spans="2:9">
       <c r="B25" s="9"/>
       <c r="C25" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D25" s="8">
         <v>8</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F25" s="8">
         <v>1</v>
@@ -4262,16 +4256,16 @@
     </row>
     <row r="26" spans="2:9">
       <c r="B26" s="14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D26" s="13">
         <v>4</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F26" s="13">
         <v>9</v>
@@ -4288,13 +4282,13 @@
     <row r="27" spans="2:9">
       <c r="B27" s="14"/>
       <c r="C27" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D27" s="13">
         <v>4</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F27" s="13">
         <v>1</v>
@@ -4312,7 +4306,7 @@
     </row>
     <row r="28" spans="2:9">
       <c r="B28" s="24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C28" s="23"/>
       <c r="D28" s="23"/>
@@ -4326,7 +4320,7 @@
     </row>
     <row r="29" spans="2:9">
       <c r="B29" s="28" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28"/>
@@ -4338,16 +4332,16 @@
     </row>
     <row r="30" spans="2:9">
       <c r="B30" s="14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D30" s="13">
         <v>37</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F30" s="13">
         <v>9</v>
@@ -4364,13 +4358,13 @@
     <row r="31" spans="2:9">
       <c r="B31" s="14"/>
       <c r="C31" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D31" s="13">
         <v>20</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F31" s="13">
         <v>1</v>
@@ -4388,16 +4382,16 @@
     </row>
     <row r="32" spans="2:9">
       <c r="B32" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D32" s="8">
         <v>5</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32" s="8">
         <v>9</v>
@@ -4414,13 +4408,13 @@
     <row r="33" spans="2:9">
       <c r="B33" s="9"/>
       <c r="C33" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D33" s="8">
         <v>4</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F33" s="8">
         <v>1</v>
@@ -4438,16 +4432,16 @@
     </row>
     <row r="34" spans="2:9">
       <c r="B34" s="14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D34" s="13">
         <v>1</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F34" s="13">
         <v>9</v>
@@ -4464,13 +4458,13 @@
     <row r="35" spans="2:9">
       <c r="B35" s="14"/>
       <c r="C35" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D35" s="13">
         <v>2</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F35" s="13">
         <v>1</v>
@@ -4488,7 +4482,7 @@
     </row>
     <row r="36" spans="2:9">
       <c r="B36" s="24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C36" s="23"/>
       <c r="D36" s="23"/>
@@ -4502,7 +4496,7 @@
     </row>
     <row r="37" spans="2:9">
       <c r="B37" s="19" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C37" s="18"/>
       <c r="D37" s="18"/>

</xml_diff>